<commit_message>
not sure what happened here. Second attempt
</commit_message>
<xml_diff>
--- a/financialPlanning.xlsx
+++ b/financialPlanning.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Description</t>
   </si>
@@ -34,6 +34,9 @@
     <t>SallieMae Loan</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>ACS Loan</t>
   </si>
   <si>
@@ -41,6 +44,27 @@
   </si>
   <si>
     <t>Sti Loan</t>
+  </si>
+  <si>
+    <t>Mortgage</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>electric</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>mastercard</t>
+  </si>
+  <si>
+    <t>earthtreks</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -54,6 +78,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -74,6 +99,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -143,20 +169,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="D12" activeCellId="0" pane="topLeft" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2" s="2">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2" s="2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -174,21 +200,113 @@
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>103.24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>132.15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>222.16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1588</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="D20" s="1" t="inlineStr">
+        <f aca="false">SUM(D2:D19)</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -209,17 +327,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -234,17 +352,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
included stuff for cell phone. Do not have up to date bill
</commit_message>
<xml_diff>
--- a/financialPlanning.xlsx
+++ b/financialPlanning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>cell phone bill</t>
   </si>
 </sst>
 </file>
@@ -430,13 +433,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.140625"/>
     <col min="2" max="3" width="11.7109375"/>
@@ -444,7 +447,7 @@
     <col min="5" max="1025" width="11.7109375"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="12.75">
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -461,7 +464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -478,7 +481,7 @@
         <v>41158</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -492,7 +495,7 @@
         <v>132.15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -506,7 +509,7 @@
         <v>222.16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -523,7 +526,7 @@
         <v>41157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="12.75">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -534,7 +537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="12.75">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -545,68 +548,79 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="12.75">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>242.02</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12.75">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="12.75">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="12.75">
-      <c r="A15" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D17" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="20" spans="3:4" ht="12.75">
-      <c r="C20" t="s">
+    <row r="22" spans="1:4">
+      <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="1">
-        <f>SUM(D2:D19)</f>
-        <v>2878.46</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4" ht="12.75">
-      <c r="C21" t="s">
+      <c r="D22" s="1">
+        <f>SUM(D2:D21)</f>
+        <v>2998.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D23" s="1">
         <v>4772</v>
       </c>
     </row>
-    <row r="22" spans="3:4" ht="12.75">
-      <c r="C22" t="s">
+    <row r="24" spans="1:4">
+      <c r="C24" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1">
-        <f>D21-D20</f>
-        <v>1893.54</v>
+      <c r="D24" s="1">
+        <f>D23-D22</f>
+        <v>1773.54</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +641,7 @@
       <selection activeCellId="1" sqref="H12:I14 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="11.7109375"/>
   </cols>
@@ -649,7 +663,7 @@
       <selection activeCellId="1" sqref="H12:I14 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1025" width="11.7109375"/>
   </cols>

</xml_diff>